<commit_message>
Solving imbalanced data problem, 1- to 3-gram BoW, add more data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1541"/>
+  <dimension ref="A1:C1724"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1486" workbookViewId="0">
-      <selection activeCell="E1503" sqref="E1503"/>
+    <sheetView tabSelected="1" topLeftCell="A1672" workbookViewId="0">
+      <selection activeCell="C1688" sqref="C1688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17323,6 +17323,2019 @@
         <v>5</v>
       </c>
     </row>
+    <row r="1542" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1542">
+        <v>31</v>
+      </c>
+      <c r="B1542">
+        <v>31</v>
+      </c>
+      <c r="C1542">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1543">
+        <v>31</v>
+      </c>
+      <c r="B1543">
+        <v>32</v>
+      </c>
+      <c r="C1543">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1544">
+        <v>31</v>
+      </c>
+      <c r="B1544">
+        <v>33</v>
+      </c>
+      <c r="C1544">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1545">
+        <v>31</v>
+      </c>
+      <c r="B1545">
+        <v>34</v>
+      </c>
+      <c r="C1545">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1546">
+        <v>31</v>
+      </c>
+      <c r="B1546">
+        <v>35</v>
+      </c>
+      <c r="C1546">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1547">
+        <v>31</v>
+      </c>
+      <c r="B1547">
+        <v>36</v>
+      </c>
+      <c r="C1547">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1548">
+        <v>31</v>
+      </c>
+      <c r="B1548">
+        <v>37</v>
+      </c>
+      <c r="C1548">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1549">
+        <v>31</v>
+      </c>
+      <c r="B1549">
+        <v>38</v>
+      </c>
+      <c r="C1549">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1550">
+        <v>31</v>
+      </c>
+      <c r="B1550">
+        <v>39</v>
+      </c>
+      <c r="C1550">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1551">
+        <v>31</v>
+      </c>
+      <c r="B1551">
+        <v>40</v>
+      </c>
+      <c r="C1551">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1552">
+        <v>31</v>
+      </c>
+      <c r="B1552">
+        <v>41</v>
+      </c>
+      <c r="C1552">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1553">
+        <v>31</v>
+      </c>
+      <c r="B1553">
+        <v>42</v>
+      </c>
+      <c r="C1553">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1554">
+        <v>31</v>
+      </c>
+      <c r="B1554">
+        <v>43</v>
+      </c>
+      <c r="C1554">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1555">
+        <v>31</v>
+      </c>
+      <c r="B1555">
+        <v>44</v>
+      </c>
+      <c r="C1555">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1556">
+        <v>31</v>
+      </c>
+      <c r="B1556">
+        <v>45</v>
+      </c>
+      <c r="C1556">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1557">
+        <v>31</v>
+      </c>
+      <c r="B1557">
+        <v>46</v>
+      </c>
+      <c r="C1557">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1558">
+        <v>31</v>
+      </c>
+      <c r="B1558">
+        <v>47</v>
+      </c>
+      <c r="C1558">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1559">
+        <v>31</v>
+      </c>
+      <c r="B1559">
+        <v>48</v>
+      </c>
+      <c r="C1559">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1560">
+        <v>31</v>
+      </c>
+      <c r="B1560">
+        <v>49</v>
+      </c>
+      <c r="C1560">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1561">
+        <v>31</v>
+      </c>
+      <c r="B1561">
+        <v>50</v>
+      </c>
+      <c r="C1561">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1562">
+        <v>31</v>
+      </c>
+      <c r="B1562">
+        <v>51</v>
+      </c>
+      <c r="C1562">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1563">
+        <v>31</v>
+      </c>
+      <c r="B1563">
+        <v>52</v>
+      </c>
+      <c r="C1563">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1564">
+        <v>31</v>
+      </c>
+      <c r="B1564">
+        <v>53</v>
+      </c>
+      <c r="C1564">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1565">
+        <v>31</v>
+      </c>
+      <c r="B1565">
+        <v>54</v>
+      </c>
+      <c r="C1565">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1566">
+        <v>31</v>
+      </c>
+      <c r="B1566">
+        <v>55</v>
+      </c>
+      <c r="C1566">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1567">
+        <v>31</v>
+      </c>
+      <c r="B1567">
+        <v>56</v>
+      </c>
+      <c r="C1567">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1568">
+        <v>31</v>
+      </c>
+      <c r="B1568">
+        <v>57</v>
+      </c>
+      <c r="C1568">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1569">
+        <v>31</v>
+      </c>
+      <c r="B1569">
+        <v>58</v>
+      </c>
+      <c r="C1569">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1570">
+        <v>31</v>
+      </c>
+      <c r="B1570">
+        <v>59</v>
+      </c>
+      <c r="C1570">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1571">
+        <v>31</v>
+      </c>
+      <c r="B1571">
+        <v>60</v>
+      </c>
+      <c r="C1571">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1572">
+        <v>32</v>
+      </c>
+      <c r="B1572">
+        <v>31</v>
+      </c>
+      <c r="C1572">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1573">
+        <v>32</v>
+      </c>
+      <c r="B1573">
+        <v>32</v>
+      </c>
+      <c r="C1573">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1574">
+        <v>32</v>
+      </c>
+      <c r="B1574">
+        <v>33</v>
+      </c>
+      <c r="C1574">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1575">
+        <v>32</v>
+      </c>
+      <c r="B1575">
+        <v>34</v>
+      </c>
+      <c r="C1575">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1576">
+        <v>32</v>
+      </c>
+      <c r="B1576">
+        <v>35</v>
+      </c>
+      <c r="C1576">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1577">
+        <v>32</v>
+      </c>
+      <c r="B1577">
+        <v>36</v>
+      </c>
+      <c r="C1577">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1578">
+        <v>32</v>
+      </c>
+      <c r="B1578">
+        <v>37</v>
+      </c>
+      <c r="C1578">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1579">
+        <v>32</v>
+      </c>
+      <c r="B1579">
+        <v>38</v>
+      </c>
+      <c r="C1579">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1580">
+        <v>32</v>
+      </c>
+      <c r="B1580">
+        <v>39</v>
+      </c>
+      <c r="C1580">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1581">
+        <v>32</v>
+      </c>
+      <c r="B1581">
+        <v>40</v>
+      </c>
+      <c r="C1581">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1582">
+        <v>32</v>
+      </c>
+      <c r="B1582">
+        <v>41</v>
+      </c>
+      <c r="C1582">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1583">
+        <v>32</v>
+      </c>
+      <c r="B1583">
+        <v>42</v>
+      </c>
+      <c r="C1583">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1584">
+        <v>32</v>
+      </c>
+      <c r="B1584">
+        <v>43</v>
+      </c>
+      <c r="C1584">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1585">
+        <v>32</v>
+      </c>
+      <c r="B1585">
+        <v>44</v>
+      </c>
+      <c r="C1585">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1586">
+        <v>32</v>
+      </c>
+      <c r="B1586">
+        <v>45</v>
+      </c>
+      <c r="C1586">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1587">
+        <v>32</v>
+      </c>
+      <c r="B1587">
+        <v>46</v>
+      </c>
+      <c r="C1587">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1588">
+        <v>32</v>
+      </c>
+      <c r="B1588">
+        <v>47</v>
+      </c>
+      <c r="C1588">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1589">
+        <v>32</v>
+      </c>
+      <c r="B1589">
+        <v>48</v>
+      </c>
+      <c r="C1589">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1590">
+        <v>32</v>
+      </c>
+      <c r="B1590">
+        <v>49</v>
+      </c>
+      <c r="C1590">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1591">
+        <v>32</v>
+      </c>
+      <c r="B1591">
+        <v>50</v>
+      </c>
+      <c r="C1591">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1592">
+        <v>32</v>
+      </c>
+      <c r="B1592">
+        <v>51</v>
+      </c>
+      <c r="C1592">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1593">
+        <v>32</v>
+      </c>
+      <c r="B1593">
+        <v>52</v>
+      </c>
+      <c r="C1593">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1594">
+        <v>32</v>
+      </c>
+      <c r="B1594">
+        <v>53</v>
+      </c>
+      <c r="C1594">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1595">
+        <v>32</v>
+      </c>
+      <c r="B1595">
+        <v>54</v>
+      </c>
+      <c r="C1595">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1596">
+        <v>32</v>
+      </c>
+      <c r="B1596">
+        <v>55</v>
+      </c>
+      <c r="C1596">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1597">
+        <v>32</v>
+      </c>
+      <c r="B1597">
+        <v>56</v>
+      </c>
+      <c r="C1597">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1598">
+        <v>32</v>
+      </c>
+      <c r="B1598">
+        <v>57</v>
+      </c>
+      <c r="C1598">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1599">
+        <v>32</v>
+      </c>
+      <c r="B1599">
+        <v>58</v>
+      </c>
+      <c r="C1599">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1600">
+        <v>32</v>
+      </c>
+      <c r="B1600">
+        <v>59</v>
+      </c>
+      <c r="C1600">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1601">
+        <v>32</v>
+      </c>
+      <c r="B1601">
+        <v>60</v>
+      </c>
+      <c r="C1601">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1602">
+        <v>34</v>
+      </c>
+      <c r="B1602">
+        <v>31</v>
+      </c>
+      <c r="C1602">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1603">
+        <v>34</v>
+      </c>
+      <c r="B1603">
+        <v>32</v>
+      </c>
+      <c r="C1603">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1604">
+        <v>34</v>
+      </c>
+      <c r="B1604">
+        <v>33</v>
+      </c>
+      <c r="C1604">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1605">
+        <v>34</v>
+      </c>
+      <c r="B1605">
+        <v>34</v>
+      </c>
+      <c r="C1605">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1606">
+        <v>34</v>
+      </c>
+      <c r="B1606">
+        <v>35</v>
+      </c>
+      <c r="C1606">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1607">
+        <v>34</v>
+      </c>
+      <c r="B1607">
+        <v>36</v>
+      </c>
+      <c r="C1607">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1608">
+        <v>34</v>
+      </c>
+      <c r="B1608">
+        <v>37</v>
+      </c>
+      <c r="C1608">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1609">
+        <v>34</v>
+      </c>
+      <c r="B1609">
+        <v>38</v>
+      </c>
+      <c r="C1609">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1610">
+        <v>34</v>
+      </c>
+      <c r="B1610">
+        <v>39</v>
+      </c>
+      <c r="C1610">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1611" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1611">
+        <v>34</v>
+      </c>
+      <c r="B1611">
+        <v>40</v>
+      </c>
+      <c r="C1611">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1612">
+        <v>34</v>
+      </c>
+      <c r="B1612">
+        <v>41</v>
+      </c>
+      <c r="C1612">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1613" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1613">
+        <v>34</v>
+      </c>
+      <c r="B1613">
+        <v>42</v>
+      </c>
+      <c r="C1613">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1614">
+        <v>34</v>
+      </c>
+      <c r="B1614">
+        <v>43</v>
+      </c>
+      <c r="C1614">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1615">
+        <v>34</v>
+      </c>
+      <c r="B1615">
+        <v>44</v>
+      </c>
+      <c r="C1615">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1616">
+        <v>34</v>
+      </c>
+      <c r="B1616">
+        <v>45</v>
+      </c>
+      <c r="C1616">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1617">
+        <v>34</v>
+      </c>
+      <c r="B1617">
+        <v>46</v>
+      </c>
+      <c r="C1617">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1618">
+        <v>34</v>
+      </c>
+      <c r="B1618">
+        <v>47</v>
+      </c>
+      <c r="C1618">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1619">
+        <v>34</v>
+      </c>
+      <c r="B1619">
+        <v>48</v>
+      </c>
+      <c r="C1619">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1620">
+        <v>34</v>
+      </c>
+      <c r="B1620">
+        <v>49</v>
+      </c>
+      <c r="C1620">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1621">
+        <v>34</v>
+      </c>
+      <c r="B1621">
+        <v>50</v>
+      </c>
+      <c r="C1621">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1622">
+        <v>34</v>
+      </c>
+      <c r="B1622">
+        <v>51</v>
+      </c>
+      <c r="C1622">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1623">
+        <v>34</v>
+      </c>
+      <c r="B1623">
+        <v>52</v>
+      </c>
+      <c r="C1623">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1624">
+        <v>34</v>
+      </c>
+      <c r="B1624">
+        <v>53</v>
+      </c>
+      <c r="C1624">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1625">
+        <v>34</v>
+      </c>
+      <c r="B1625">
+        <v>54</v>
+      </c>
+      <c r="C1625">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1626">
+        <v>34</v>
+      </c>
+      <c r="B1626">
+        <v>55</v>
+      </c>
+      <c r="C1626">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1627">
+        <v>34</v>
+      </c>
+      <c r="B1627">
+        <v>56</v>
+      </c>
+      <c r="C1627">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1628">
+        <v>34</v>
+      </c>
+      <c r="B1628">
+        <v>57</v>
+      </c>
+      <c r="C1628">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1629">
+        <v>34</v>
+      </c>
+      <c r="B1629">
+        <v>58</v>
+      </c>
+      <c r="C1629">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1630">
+        <v>34</v>
+      </c>
+      <c r="B1630">
+        <v>59</v>
+      </c>
+      <c r="C1630">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1631" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1631">
+        <v>34</v>
+      </c>
+      <c r="B1631">
+        <v>60</v>
+      </c>
+      <c r="C1631">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1632">
+        <v>33</v>
+      </c>
+      <c r="B1632">
+        <v>31</v>
+      </c>
+      <c r="C1632">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1633" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1633">
+        <v>33</v>
+      </c>
+      <c r="B1633">
+        <v>32</v>
+      </c>
+      <c r="C1633">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1634">
+        <v>33</v>
+      </c>
+      <c r="B1634">
+        <v>33</v>
+      </c>
+      <c r="C1634">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1635">
+        <v>33</v>
+      </c>
+      <c r="B1635">
+        <v>34</v>
+      </c>
+      <c r="C1635">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1636">
+        <v>33</v>
+      </c>
+      <c r="B1636">
+        <v>35</v>
+      </c>
+      <c r="C1636">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1637">
+        <v>33</v>
+      </c>
+      <c r="B1637">
+        <v>36</v>
+      </c>
+      <c r="C1637">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1638">
+        <v>33</v>
+      </c>
+      <c r="B1638">
+        <v>37</v>
+      </c>
+      <c r="C1638">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1639">
+        <v>33</v>
+      </c>
+      <c r="B1639">
+        <v>38</v>
+      </c>
+      <c r="C1639">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1640">
+        <v>33</v>
+      </c>
+      <c r="B1640">
+        <v>39</v>
+      </c>
+      <c r="C1640">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1641">
+        <v>33</v>
+      </c>
+      <c r="B1641">
+        <v>40</v>
+      </c>
+      <c r="C1641">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1642">
+        <v>33</v>
+      </c>
+      <c r="B1642">
+        <v>41</v>
+      </c>
+      <c r="C1642">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1643">
+        <v>33</v>
+      </c>
+      <c r="B1643">
+        <v>42</v>
+      </c>
+      <c r="C1643">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1644">
+        <v>33</v>
+      </c>
+      <c r="B1644">
+        <v>43</v>
+      </c>
+      <c r="C1644">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1645">
+        <v>33</v>
+      </c>
+      <c r="B1645">
+        <v>44</v>
+      </c>
+      <c r="C1645">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1646">
+        <v>33</v>
+      </c>
+      <c r="B1646">
+        <v>45</v>
+      </c>
+      <c r="C1646">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1647">
+        <v>33</v>
+      </c>
+      <c r="B1647">
+        <v>46</v>
+      </c>
+      <c r="C1647">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1648">
+        <v>33</v>
+      </c>
+      <c r="B1648">
+        <v>47</v>
+      </c>
+      <c r="C1648">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1649">
+        <v>33</v>
+      </c>
+      <c r="B1649">
+        <v>48</v>
+      </c>
+      <c r="C1649">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1650">
+        <v>33</v>
+      </c>
+      <c r="B1650">
+        <v>49</v>
+      </c>
+      <c r="C1650">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1651">
+        <v>33</v>
+      </c>
+      <c r="B1651">
+        <v>50</v>
+      </c>
+      <c r="C1651">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1652">
+        <v>33</v>
+      </c>
+      <c r="B1652">
+        <v>51</v>
+      </c>
+      <c r="C1652">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1653">
+        <v>33</v>
+      </c>
+      <c r="B1653">
+        <v>52</v>
+      </c>
+      <c r="C1653">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1654">
+        <v>33</v>
+      </c>
+      <c r="B1654">
+        <v>53</v>
+      </c>
+      <c r="C1654">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1655">
+        <v>33</v>
+      </c>
+      <c r="B1655">
+        <v>54</v>
+      </c>
+      <c r="C1655">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1656">
+        <v>33</v>
+      </c>
+      <c r="B1656">
+        <v>55</v>
+      </c>
+      <c r="C1656">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1657">
+        <v>33</v>
+      </c>
+      <c r="B1657">
+        <v>56</v>
+      </c>
+      <c r="C1657">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1658">
+        <v>33</v>
+      </c>
+      <c r="B1658">
+        <v>57</v>
+      </c>
+      <c r="C1658">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1659">
+        <v>33</v>
+      </c>
+      <c r="B1659">
+        <v>58</v>
+      </c>
+      <c r="C1659">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1660">
+        <v>33</v>
+      </c>
+      <c r="B1660">
+        <v>59</v>
+      </c>
+      <c r="C1660">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1661">
+        <v>33</v>
+      </c>
+      <c r="B1661">
+        <v>60</v>
+      </c>
+      <c r="C1661">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1662">
+        <v>35</v>
+      </c>
+      <c r="B1662">
+        <v>31</v>
+      </c>
+      <c r="C1662">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1663">
+        <v>35</v>
+      </c>
+      <c r="B1663">
+        <v>32</v>
+      </c>
+      <c r="C1663">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1664">
+        <v>35</v>
+      </c>
+      <c r="B1664">
+        <v>33</v>
+      </c>
+      <c r="C1664">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1665">
+        <v>35</v>
+      </c>
+      <c r="B1665">
+        <v>34</v>
+      </c>
+      <c r="C1665">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1666">
+        <v>35</v>
+      </c>
+      <c r="B1666">
+        <v>35</v>
+      </c>
+      <c r="C1666">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1667">
+        <v>35</v>
+      </c>
+      <c r="B1667">
+        <v>36</v>
+      </c>
+      <c r="C1667">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1668">
+        <v>35</v>
+      </c>
+      <c r="B1668">
+        <v>37</v>
+      </c>
+      <c r="C1668">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1669">
+        <v>35</v>
+      </c>
+      <c r="B1669">
+        <v>38</v>
+      </c>
+      <c r="C1669">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1670">
+        <v>35</v>
+      </c>
+      <c r="B1670">
+        <v>39</v>
+      </c>
+      <c r="C1670">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1671">
+        <v>35</v>
+      </c>
+      <c r="B1671">
+        <v>40</v>
+      </c>
+      <c r="C1671">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1672">
+        <v>35</v>
+      </c>
+      <c r="B1672">
+        <v>41</v>
+      </c>
+      <c r="C1672">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1673">
+        <v>35</v>
+      </c>
+      <c r="B1673">
+        <v>42</v>
+      </c>
+      <c r="C1673">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1674">
+        <v>35</v>
+      </c>
+      <c r="B1674">
+        <v>43</v>
+      </c>
+      <c r="C1674">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1675">
+        <v>35</v>
+      </c>
+      <c r="B1675">
+        <v>44</v>
+      </c>
+      <c r="C1675">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1676">
+        <v>35</v>
+      </c>
+      <c r="B1676">
+        <v>45</v>
+      </c>
+      <c r="C1676">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1677">
+        <v>35</v>
+      </c>
+      <c r="B1677">
+        <v>46</v>
+      </c>
+      <c r="C1677">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1678">
+        <v>35</v>
+      </c>
+      <c r="B1678">
+        <v>47</v>
+      </c>
+      <c r="C1678">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1679">
+        <v>35</v>
+      </c>
+      <c r="B1679">
+        <v>48</v>
+      </c>
+      <c r="C1679">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1680">
+        <v>35</v>
+      </c>
+      <c r="B1680">
+        <v>49</v>
+      </c>
+      <c r="C1680">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1681">
+        <v>35</v>
+      </c>
+      <c r="B1681">
+        <v>50</v>
+      </c>
+      <c r="C1681">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1682">
+        <v>35</v>
+      </c>
+      <c r="B1682">
+        <v>51</v>
+      </c>
+      <c r="C1682">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1683">
+        <v>35</v>
+      </c>
+      <c r="B1683">
+        <v>52</v>
+      </c>
+      <c r="C1683">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1684">
+        <v>35</v>
+      </c>
+      <c r="B1684">
+        <v>53</v>
+      </c>
+      <c r="C1684">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1685">
+        <v>35</v>
+      </c>
+      <c r="B1685">
+        <v>54</v>
+      </c>
+      <c r="C1685">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1686">
+        <v>35</v>
+      </c>
+      <c r="B1686">
+        <v>55</v>
+      </c>
+      <c r="C1686">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1687">
+        <v>35</v>
+      </c>
+      <c r="B1687">
+        <v>56</v>
+      </c>
+      <c r="C1687">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1688">
+        <v>35</v>
+      </c>
+      <c r="B1688">
+        <v>57</v>
+      </c>
+      <c r="C1688">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1689">
+        <v>35</v>
+      </c>
+      <c r="B1689">
+        <v>58</v>
+      </c>
+      <c r="C1689">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1690">
+        <v>35</v>
+      </c>
+      <c r="B1690">
+        <v>59</v>
+      </c>
+      <c r="C1690">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1691">
+        <v>35</v>
+      </c>
+      <c r="B1691">
+        <v>60</v>
+      </c>
+      <c r="C1691">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1692">
+        <v>36</v>
+      </c>
+      <c r="B1692">
+        <v>24</v>
+      </c>
+      <c r="C1692">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1693">
+        <v>37</v>
+      </c>
+      <c r="B1693">
+        <v>24</v>
+      </c>
+      <c r="C1693">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1694">
+        <v>38</v>
+      </c>
+      <c r="B1694">
+        <v>24</v>
+      </c>
+      <c r="C1694">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1695">
+        <v>39</v>
+      </c>
+      <c r="B1695">
+        <v>24</v>
+      </c>
+      <c r="C1695">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1696">
+        <v>40</v>
+      </c>
+      <c r="B1696">
+        <v>24</v>
+      </c>
+      <c r="C1696">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1697">
+        <v>36</v>
+      </c>
+      <c r="B1697">
+        <v>96</v>
+      </c>
+      <c r="C1697">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1698">
+        <v>36</v>
+      </c>
+      <c r="B1698">
+        <v>97</v>
+      </c>
+      <c r="C1698">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1699">
+        <v>36</v>
+      </c>
+      <c r="B1699">
+        <v>98</v>
+      </c>
+      <c r="C1699">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1700">
+        <v>36</v>
+      </c>
+      <c r="B1700">
+        <v>99</v>
+      </c>
+      <c r="C1700">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1701">
+        <v>36</v>
+      </c>
+      <c r="B1701">
+        <v>100</v>
+      </c>
+      <c r="C1701">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1702">
+        <v>37</v>
+      </c>
+      <c r="B1702">
+        <v>96</v>
+      </c>
+      <c r="C1702">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1703">
+        <v>37</v>
+      </c>
+      <c r="B1703">
+        <v>97</v>
+      </c>
+      <c r="C1703">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1704">
+        <v>37</v>
+      </c>
+      <c r="B1704">
+        <v>98</v>
+      </c>
+      <c r="C1704">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1705">
+        <v>37</v>
+      </c>
+      <c r="B1705">
+        <v>99</v>
+      </c>
+      <c r="C1705">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1706">
+        <v>37</v>
+      </c>
+      <c r="B1706">
+        <v>100</v>
+      </c>
+      <c r="C1706">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1707">
+        <v>38</v>
+      </c>
+      <c r="B1707">
+        <v>96</v>
+      </c>
+      <c r="C1707">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1708">
+        <v>38</v>
+      </c>
+      <c r="B1708">
+        <v>97</v>
+      </c>
+      <c r="C1708">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1709">
+        <v>38</v>
+      </c>
+      <c r="B1709">
+        <v>98</v>
+      </c>
+      <c r="C1709">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1710">
+        <v>38</v>
+      </c>
+      <c r="B1710">
+        <v>99</v>
+      </c>
+      <c r="C1710">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1711">
+        <v>38</v>
+      </c>
+      <c r="B1711">
+        <v>100</v>
+      </c>
+      <c r="C1711">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1712">
+        <v>39</v>
+      </c>
+      <c r="B1712">
+        <v>96</v>
+      </c>
+      <c r="C1712">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1713">
+        <v>39</v>
+      </c>
+      <c r="B1713">
+        <v>97</v>
+      </c>
+      <c r="C1713">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1714">
+        <v>39</v>
+      </c>
+      <c r="B1714">
+        <v>98</v>
+      </c>
+      <c r="C1714">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1715">
+        <v>39</v>
+      </c>
+      <c r="B1715">
+        <v>99</v>
+      </c>
+      <c r="C1715">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1716">
+        <v>39</v>
+      </c>
+      <c r="B1716">
+        <v>100</v>
+      </c>
+      <c r="C1716">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1717">
+        <v>40</v>
+      </c>
+      <c r="B1717">
+        <v>96</v>
+      </c>
+      <c r="C1717">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1718">
+        <v>40</v>
+      </c>
+      <c r="B1718">
+        <v>97</v>
+      </c>
+      <c r="C1718">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1719">
+        <v>40</v>
+      </c>
+      <c r="B1719">
+        <v>98</v>
+      </c>
+      <c r="C1719">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1720">
+        <v>40</v>
+      </c>
+      <c r="B1720">
+        <v>99</v>
+      </c>
+      <c r="C1720">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1721">
+        <v>40</v>
+      </c>
+      <c r="B1721">
+        <v>100</v>
+      </c>
+      <c r="C1721">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1722">
+        <v>46</v>
+      </c>
+      <c r="B1722">
+        <v>21</v>
+      </c>
+      <c r="C1722">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1723">
+        <v>46</v>
+      </c>
+      <c r="B1723">
+        <v>27</v>
+      </c>
+      <c r="C1723">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1724">
+        <v>46</v>
+      </c>
+      <c r="B1724">
+        <v>48</v>
+      </c>
+      <c r="C1724">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Downsampling, LSTM and CNN architecture update
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -364,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1920"/>
+  <dimension ref="A1:C2000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1888" workbookViewId="0">
-      <selection activeCell="C1910" sqref="C1910"/>
+    <sheetView tabSelected="1" topLeftCell="A1909" workbookViewId="0">
+      <selection activeCell="C1923" sqref="C1923"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21492,7 +21493,657 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1921" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1921">
+        <v>36</v>
+      </c>
+      <c r="B1921">
+        <v>71</v>
+      </c>
+      <c r="C1921">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1922" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1922">
+        <v>36</v>
+      </c>
+      <c r="B1922">
+        <v>72</v>
+      </c>
+      <c r="C1922">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1923" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1923">
+        <v>36</v>
+      </c>
+      <c r="B1923">
+        <v>73</v>
+      </c>
+      <c r="C1923">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1924" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1924">
+        <v>36</v>
+      </c>
+      <c r="B1924">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1925" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1925">
+        <v>36</v>
+      </c>
+      <c r="B1925">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1926" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1926">
+        <v>36</v>
+      </c>
+      <c r="B1926">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1927" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1927">
+        <v>36</v>
+      </c>
+      <c r="B1927">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="1928" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1928">
+        <v>36</v>
+      </c>
+      <c r="B1928">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="1929" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1929">
+        <v>36</v>
+      </c>
+      <c r="B1929">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1930" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1930">
+        <v>36</v>
+      </c>
+      <c r="B1930">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1931" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1931">
+        <v>37</v>
+      </c>
+      <c r="B1931">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="1932" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1932">
+        <v>37</v>
+      </c>
+      <c r="B1932">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="1933" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1933">
+        <v>37</v>
+      </c>
+      <c r="B1933">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1934" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1934">
+        <v>37</v>
+      </c>
+      <c r="B1934">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1935" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1935">
+        <v>37</v>
+      </c>
+      <c r="B1935">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1936" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1936">
+        <v>37</v>
+      </c>
+      <c r="B1936">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1937" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1937">
+        <v>37</v>
+      </c>
+      <c r="B1937">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="1938" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1938">
+        <v>37</v>
+      </c>
+      <c r="B1938">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="1939" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1939">
+        <v>37</v>
+      </c>
+      <c r="B1939">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1940" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1940">
+        <v>37</v>
+      </c>
+      <c r="B1940">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1941" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1941">
+        <v>38</v>
+      </c>
+      <c r="B1941">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="1942" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1942">
+        <v>38</v>
+      </c>
+      <c r="B1942">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="1943" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1943">
+        <v>38</v>
+      </c>
+      <c r="B1943">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1944" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1944">
+        <v>38</v>
+      </c>
+      <c r="B1944">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1945" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1945">
+        <v>38</v>
+      </c>
+      <c r="B1945">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1946" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1946">
+        <v>38</v>
+      </c>
+      <c r="B1946">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1947">
+        <v>38</v>
+      </c>
+      <c r="B1947">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="1948" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1948">
+        <v>38</v>
+      </c>
+      <c r="B1948">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="1949" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1949">
+        <v>38</v>
+      </c>
+      <c r="B1949">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1950" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1950">
+        <v>38</v>
+      </c>
+      <c r="B1950">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1951" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1951">
+        <v>39</v>
+      </c>
+      <c r="B1951">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="1952" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1952">
+        <v>39</v>
+      </c>
+      <c r="B1952">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="1953" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1953">
+        <v>39</v>
+      </c>
+      <c r="B1953">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1954" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1954">
+        <v>39</v>
+      </c>
+      <c r="B1954">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1955" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1955">
+        <v>39</v>
+      </c>
+      <c r="B1955">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1956" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1956">
+        <v>39</v>
+      </c>
+      <c r="B1956">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1957" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1957">
+        <v>39</v>
+      </c>
+      <c r="B1957">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="1958" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1958">
+        <v>39</v>
+      </c>
+      <c r="B1958">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="1959" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1959">
+        <v>39</v>
+      </c>
+      <c r="B1959">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1960" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1960">
+        <v>39</v>
+      </c>
+      <c r="B1960">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1961" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1961">
+        <v>40</v>
+      </c>
+      <c r="B1961">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="1962" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1962">
+        <v>40</v>
+      </c>
+      <c r="B1962">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="1963" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1963">
+        <v>40</v>
+      </c>
+      <c r="B1963">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1964" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1964">
+        <v>40</v>
+      </c>
+      <c r="B1964">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1965" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1965">
+        <v>40</v>
+      </c>
+      <c r="B1965">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1966" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1966">
+        <v>40</v>
+      </c>
+      <c r="B1966">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1967" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1967">
+        <v>40</v>
+      </c>
+      <c r="B1967">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="1968" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1968">
+        <v>40</v>
+      </c>
+      <c r="B1968">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="1969" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1969">
+        <v>40</v>
+      </c>
+      <c r="B1969">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1970" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1970">
+        <v>40</v>
+      </c>
+      <c r="B1970">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1971" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1971">
+        <v>44</v>
+      </c>
+      <c r="B1971">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="1972" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1972">
+        <v>44</v>
+      </c>
+      <c r="B1972">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="1973" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1973">
+        <v>44</v>
+      </c>
+      <c r="B1973">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1974" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1974">
+        <v>44</v>
+      </c>
+      <c r="B1974">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1975" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1975">
+        <v>44</v>
+      </c>
+      <c r="B1975">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1976" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1976">
+        <v>44</v>
+      </c>
+      <c r="B1976">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1977" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1977">
+        <v>44</v>
+      </c>
+      <c r="B1977">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="1978" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1978">
+        <v>44</v>
+      </c>
+      <c r="B1978">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="1979" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1979">
+        <v>44</v>
+      </c>
+      <c r="B1979">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1980" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1980">
+        <v>44</v>
+      </c>
+      <c r="B1980">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1981" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1981">
+        <v>45</v>
+      </c>
+      <c r="B1981">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="1982" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1982">
+        <v>45</v>
+      </c>
+      <c r="B1982">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="1983" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1983">
+        <v>45</v>
+      </c>
+      <c r="B1983">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1984" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1984">
+        <v>45</v>
+      </c>
+      <c r="B1984">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1985" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1985">
+        <v>45</v>
+      </c>
+      <c r="B1985">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1986" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1986">
+        <v>45</v>
+      </c>
+      <c r="B1986">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1987" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1987">
+        <v>45</v>
+      </c>
+      <c r="B1987">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="1988" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1988">
+        <v>45</v>
+      </c>
+      <c r="B1988">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="1989" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1989">
+        <v>45</v>
+      </c>
+      <c r="B1989">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1990" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1990">
+        <v>45</v>
+      </c>
+      <c r="B1990">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1991" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1991">
+        <v>52</v>
+      </c>
+      <c r="B1991">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="1992" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1992">
+        <v>52</v>
+      </c>
+      <c r="B1992">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="1993" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1993">
+        <v>52</v>
+      </c>
+      <c r="B1993">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1994" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1994">
+        <v>52</v>
+      </c>
+      <c r="B1994">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1995" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1995">
+        <v>52</v>
+      </c>
+      <c r="B1995">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1996" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1996">
+        <v>52</v>
+      </c>
+      <c r="B1996">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1997" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1997">
+        <v>52</v>
+      </c>
+      <c r="B1997">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="1998" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1998">
+        <v>52</v>
+      </c>
+      <c r="B1998">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="1999" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1999">
+        <v>52</v>
+      </c>
+      <c r="B1999">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2000" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2000">
+        <v>52</v>
+      </c>
+      <c r="B2000">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed resume-matching implementation to continuous data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -47,7 +46,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -55,12 +54,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -367,8 +384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1909" workbookViewId="0">
-      <selection activeCell="C1923" sqref="C1923"/>
+    <sheetView tabSelected="1" topLeftCell="A1912" workbookViewId="0">
+      <selection activeCell="A1924" sqref="A1924:C2000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21515,7 +21532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1923" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1923" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1923">
         <v>36</v>
       </c>
@@ -21526,620 +21543,851 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1924" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1924">
+    <row r="1924" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1924" s="1">
         <v>36</v>
       </c>
-      <c r="B1924">
+      <c r="B1924" s="1">
+        <v>71</v>
+      </c>
+      <c r="C1924" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1925" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1925" s="1">
+        <v>36</v>
+      </c>
+      <c r="B1925" s="1">
+        <v>72</v>
+      </c>
+      <c r="C1925" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1926" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1926" s="1">
+        <v>36</v>
+      </c>
+      <c r="B1926" s="1">
+        <v>73</v>
+      </c>
+      <c r="C1926" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1927" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1927" s="1">
+        <v>36</v>
+      </c>
+      <c r="B1927" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="1925" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1925">
+      <c r="C1927" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1928" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1928" s="1">
         <v>36</v>
       </c>
-      <c r="B1925">
+      <c r="B1928" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="1926" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1926">
+      <c r="C1928" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1929" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1929" s="1">
         <v>36</v>
       </c>
-      <c r="B1926">
+      <c r="B1929" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="1927" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1927">
+      <c r="C1929" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1930" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1930" s="1">
         <v>36</v>
       </c>
-      <c r="B1927">
+      <c r="B1930" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="1928" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1928">
+      <c r="C1930" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1931" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1931" s="1">
         <v>36</v>
       </c>
-      <c r="B1928">
+      <c r="B1931" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="1929" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1929">
+      <c r="C1931" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1932" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1932" s="1">
         <v>36</v>
       </c>
-      <c r="B1929">
+      <c r="B1932" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="1930" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1930">
+      <c r="C1932" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1933" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1933" s="1">
         <v>36</v>
       </c>
-      <c r="B1930">
+      <c r="B1933" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="1931" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1931">
+      <c r="C1933" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1934" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1934" s="1">
         <v>37</v>
       </c>
-      <c r="B1931">
+      <c r="B1934" s="1">
         <v>71</v>
       </c>
-    </row>
-    <row r="1932" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1932">
+      <c r="C1934" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1935" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1935" s="1">
         <v>37</v>
       </c>
-      <c r="B1932">
+      <c r="B1935" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="1933" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1933">
+      <c r="C1935" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1936" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1936" s="1">
         <v>37</v>
       </c>
-      <c r="B1933">
+      <c r="B1936" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="1934" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1934">
+      <c r="C1936" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1937" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1937" s="1">
         <v>37</v>
       </c>
-      <c r="B1934">
+      <c r="B1937" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="1935" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1935">
+      <c r="C1937" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1938" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1938" s="1">
         <v>37</v>
       </c>
-      <c r="B1935">
+      <c r="B1938" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="1936" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1936">
+      <c r="C1938" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1939" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1939" s="1">
         <v>37</v>
       </c>
-      <c r="B1936">
+      <c r="B1939" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="1937" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1937">
+      <c r="C1939" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1940" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1940" s="1">
         <v>37</v>
       </c>
-      <c r="B1937">
+      <c r="B1940" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="1938" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1938">
+      <c r="C1940" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1941" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1941" s="1">
         <v>37</v>
       </c>
-      <c r="B1938">
+      <c r="B1941" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="1939" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1939">
+      <c r="C1941" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1942" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1942" s="1">
         <v>37</v>
       </c>
-      <c r="B1939">
+      <c r="B1942" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="1940" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1940">
+      <c r="C1942" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1943" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1943" s="1">
         <v>37</v>
       </c>
-      <c r="B1940">
+      <c r="B1943" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="1941" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1941">
+      <c r="C1943" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1944" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1944" s="1">
         <v>38</v>
       </c>
-      <c r="B1941">
+      <c r="B1944" s="1">
         <v>71</v>
       </c>
-    </row>
-    <row r="1942" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1942">
+      <c r="C1944" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1945" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1945" s="1">
         <v>38</v>
       </c>
-      <c r="B1942">
+      <c r="B1945" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="1943" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1943">
+      <c r="C1945" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1946" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1946" s="1">
         <v>38</v>
       </c>
-      <c r="B1943">
+      <c r="B1946" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="1944" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1944">
+      <c r="C1946" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1947" s="1">
         <v>38</v>
       </c>
-      <c r="B1944">
+      <c r="B1947" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="1945" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1945">
+      <c r="C1947" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1948" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1948" s="1">
         <v>38</v>
       </c>
-      <c r="B1945">
+      <c r="B1948" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="1946" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1946">
+      <c r="C1948" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1949" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1949" s="1">
         <v>38</v>
       </c>
-      <c r="B1946">
+      <c r="B1949" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="1947" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1947">
+      <c r="C1949" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1950" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1950" s="1">
         <v>38</v>
       </c>
-      <c r="B1947">
+      <c r="B1950" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="1948" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1948">
+      <c r="C1950" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1951" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1951" s="1">
         <v>38</v>
       </c>
-      <c r="B1948">
+      <c r="B1951" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="1949" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1949">
+      <c r="C1951" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1952" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1952" s="1">
         <v>38</v>
       </c>
-      <c r="B1949">
+      <c r="B1952" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="1950" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1950">
+      <c r="C1952" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1953" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1953" s="1">
         <v>38</v>
       </c>
-      <c r="B1950">
+      <c r="B1953" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="1951" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1951">
+      <c r="C1953" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1954" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1954" s="1">
         <v>39</v>
       </c>
-      <c r="B1951">
+      <c r="B1954" s="1">
         <v>71</v>
       </c>
-    </row>
-    <row r="1952" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1952">
+      <c r="C1954" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1955" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1955" s="1">
         <v>39</v>
       </c>
-      <c r="B1952">
+      <c r="B1955" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="1953" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1953">
+      <c r="C1955" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1956" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1956" s="1">
         <v>39</v>
       </c>
-      <c r="B1953">
+      <c r="B1956" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="1954" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1954">
+      <c r="C1956" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1957" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1957" s="1">
         <v>39</v>
       </c>
-      <c r="B1954">
+      <c r="B1957" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="1955" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1955">
+      <c r="C1957" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1958" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1958" s="1">
         <v>39</v>
       </c>
-      <c r="B1955">
+      <c r="B1958" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="1956" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1956">
+      <c r="C1958" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1959" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1959" s="1">
         <v>39</v>
       </c>
-      <c r="B1956">
+      <c r="B1959" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="1957" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1957">
+      <c r="C1959" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1960" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1960" s="1">
         <v>39</v>
       </c>
-      <c r="B1957">
+      <c r="B1960" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="1958" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1958">
+      <c r="C1960" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1961" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1961" s="1">
         <v>39</v>
       </c>
-      <c r="B1958">
+      <c r="B1961" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="1959" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1959">
+      <c r="C1961" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1962" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1962" s="1">
         <v>39</v>
       </c>
-      <c r="B1959">
+      <c r="B1962" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="1960" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1960">
+      <c r="C1962" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1963" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1963" s="1">
         <v>39</v>
       </c>
-      <c r="B1960">
+      <c r="B1963" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="1961" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1961">
+      <c r="C1963" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1964" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1964" s="1">
         <v>40</v>
       </c>
-      <c r="B1961">
+      <c r="B1964" s="1">
         <v>71</v>
       </c>
-    </row>
-    <row r="1962" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1962">
+      <c r="C1964" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1965" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1965" s="1">
         <v>40</v>
       </c>
-      <c r="B1962">
+      <c r="B1965" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="1963" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1963">
+      <c r="C1965" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1966" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1966" s="1">
         <v>40</v>
       </c>
-      <c r="B1963">
+      <c r="B1966" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="1964" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1964">
+      <c r="C1966" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1967" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1967" s="1">
         <v>40</v>
       </c>
-      <c r="B1964">
+      <c r="B1967" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="1965" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1965">
+      <c r="C1967" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1968" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1968" s="1">
         <v>40</v>
       </c>
-      <c r="B1965">
+      <c r="B1968" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="1966" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1966">
+      <c r="C1968" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1969" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1969" s="1">
         <v>40</v>
       </c>
-      <c r="B1966">
+      <c r="B1969" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="1967" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1967">
+      <c r="C1969" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1970" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1970" s="1">
         <v>40</v>
       </c>
-      <c r="B1967">
+      <c r="B1970" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="1968" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1968">
+      <c r="C1970" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1971" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1971" s="1">
         <v>40</v>
       </c>
-      <c r="B1968">
+      <c r="B1971" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="1969" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1969">
+      <c r="C1971" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1972" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1972" s="1">
         <v>40</v>
       </c>
-      <c r="B1969">
+      <c r="B1972" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="1970" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1970">
+      <c r="C1972" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1973" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1973" s="1">
         <v>40</v>
       </c>
-      <c r="B1970">
+      <c r="B1973" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="1971" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1971">
+      <c r="C1973" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1974" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1974" s="1">
         <v>44</v>
       </c>
-      <c r="B1971">
+      <c r="B1974" s="1">
         <v>71</v>
       </c>
-    </row>
-    <row r="1972" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1972">
+      <c r="C1974" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1975" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1975" s="1">
         <v>44</v>
       </c>
-      <c r="B1972">
+      <c r="B1975" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="1973" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1973">
+      <c r="C1975" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1976" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1976" s="1">
         <v>44</v>
       </c>
-      <c r="B1973">
+      <c r="B1976" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="1974" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1974">
+      <c r="C1976" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1977" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1977" s="1">
         <v>44</v>
       </c>
-      <c r="B1974">
+      <c r="B1977" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="1975" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1975">
+      <c r="C1977" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1978" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1978" s="1">
         <v>44</v>
       </c>
-      <c r="B1975">
+      <c r="B1978" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="1976" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1976">
+      <c r="C1978" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1979" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1979" s="1">
         <v>44</v>
       </c>
-      <c r="B1976">
+      <c r="B1979" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="1977" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1977">
+      <c r="C1979" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1980" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1980" s="1">
         <v>44</v>
       </c>
-      <c r="B1977">
+      <c r="B1980" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="1978" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1978">
+      <c r="C1980" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1981" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1981" s="1">
         <v>44</v>
       </c>
-      <c r="B1978">
+      <c r="B1981" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="1979" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1979">
+      <c r="C1981" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1982" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1982" s="1">
         <v>44</v>
       </c>
-      <c r="B1979">
+      <c r="B1982" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="1980" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1980">
+      <c r="C1982" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1983" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1983" s="1">
         <v>44</v>
       </c>
-      <c r="B1980">
+      <c r="B1983" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="1981" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1981">
+      <c r="C1983" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1984" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1984" s="1">
         <v>45</v>
       </c>
-      <c r="B1981">
+      <c r="B1984" s="1">
         <v>71</v>
       </c>
-    </row>
-    <row r="1982" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1982">
+      <c r="C1984" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1985" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1985" s="1">
         <v>45</v>
       </c>
-      <c r="B1982">
+      <c r="B1985" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="1983" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1983">
+      <c r="C1985" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1986" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1986" s="1">
         <v>45</v>
       </c>
-      <c r="B1983">
+      <c r="B1986" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="1984" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1984">
+      <c r="C1986" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1987" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1987" s="1">
         <v>45</v>
       </c>
-      <c r="B1984">
+      <c r="B1987" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="1985" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1985">
+      <c r="C1987" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1988" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1988" s="1">
         <v>45</v>
       </c>
-      <c r="B1985">
+      <c r="B1988" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="1986" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1986">
+      <c r="C1988" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1989" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1989" s="1">
         <v>45</v>
       </c>
-      <c r="B1986">
+      <c r="B1989" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="1987" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1987">
+      <c r="C1989" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1990" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1990" s="1">
         <v>45</v>
       </c>
-      <c r="B1987">
+      <c r="B1990" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="1988" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1988">
+      <c r="C1990" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1991" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1991" s="1">
         <v>45</v>
       </c>
-      <c r="B1988">
+      <c r="B1991" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="1989" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1989">
+      <c r="C1991" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1992" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1992" s="1">
         <v>45</v>
       </c>
-      <c r="B1989">
+      <c r="B1992" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="1990" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1990">
+      <c r="C1992" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1993" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1993" s="1">
         <v>45</v>
       </c>
-      <c r="B1990">
+      <c r="B1993" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="1991" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1991">
-        <v>52</v>
-      </c>
-      <c r="B1991">
+      <c r="C1993" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1994" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1994" s="1">
+        <v>58</v>
+      </c>
+      <c r="B1994" s="1">
         <v>71</v>
       </c>
-    </row>
-    <row r="1992" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1992">
-        <v>52</v>
-      </c>
-      <c r="B1992">
+      <c r="C1994" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1995" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1995" s="1">
+        <v>58</v>
+      </c>
+      <c r="B1995" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="1993" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1993">
-        <v>52</v>
-      </c>
-      <c r="B1993">
+      <c r="C1995" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1996" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1996" s="1">
+        <v>58</v>
+      </c>
+      <c r="B1996" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="1994" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1994">
-        <v>52</v>
-      </c>
-      <c r="B1994">
+      <c r="C1996" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1997" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1997" s="1">
+        <v>58</v>
+      </c>
+      <c r="B1997" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="1995" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1995">
-        <v>52</v>
-      </c>
-      <c r="B1995">
+      <c r="C1997" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1998" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1998" s="1">
+        <v>58</v>
+      </c>
+      <c r="B1998" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="1996" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1996">
-        <v>52</v>
-      </c>
-      <c r="B1996">
+      <c r="C1998" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1999" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1999" s="1">
+        <v>58</v>
+      </c>
+      <c r="B1999" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="1997" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1997">
-        <v>52</v>
-      </c>
-      <c r="B1997">
+      <c r="C1999" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2000" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2000" s="1">
+        <v>58</v>
+      </c>
+      <c r="B2000" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="1998" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1998">
-        <v>52</v>
-      </c>
-      <c r="B1998">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="1999" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1999">
-        <v>52</v>
-      </c>
-      <c r="B1999">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2000" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2000">
-        <v>52</v>
-      </c>
-      <c r="B2000">
-        <v>80</v>
+      <c r="C2000" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>